<commit_message>
Aggiornato data.json con il caso id 36; Aggiornato il report; Caricato il PDF per il caso id 36
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LIS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LIS/V.2.0/report-checklist.xlsx
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
   <si>
     <t>NOME FORNITORE:</t>
+  </si>
+  <si>
+    <t>GESAN SRL</t>
   </si>
   <si>
     <t>IDENTIFICATIVI SOFTWARE</t>
@@ -333,13 +336,13 @@
     </r>
   </si>
   <si>
-    <t>10:28:00</t>
+    <t>10:36:00</t>
   </si>
   <si>
-    <t>35bb18b2661ea625</t>
+    <t>fec36cd913d14a73</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150201.ca4ab4f286fec1cdb3468100758c991af3551d627dbf2eeb21b2dc1d11c04c05.b583bf0275^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.f1e497be9949acc3f3de5928e179f0e15fd9febfe52158f4b6f02590c3a31589.5b86e33db0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>L’applicativo risponde con un codice di errore e il messaggio “Campo token JWT non valido” seguito dal motivo dell’errore. Il referto non viene prodotto</t>
@@ -872,7 +875,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -908,6 +911,9 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -2224,9 +2230,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="C2" t="s" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
       <c r="H2" s="4"/>
@@ -2244,15 +2252,15 @@
       <c r="T2" s="6"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" t="s" s="16">
+      <c r="A3" t="s" s="15">
         <v>2</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" t="s" s="17">
+        <v>3</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
       <c r="H3" s="4"/>
@@ -2270,13 +2278,13 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" t="s" s="16">
-        <v>3</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" t="s" s="17">
+        <v>4</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="4"/>
@@ -2294,13 +2302,13 @@
       <c r="T4" s="6"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" t="s" s="16">
-        <v>4</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" t="s" s="17">
+        <v>5</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
@@ -2318,10 +2326,10 @@
       <c r="T5" s="6"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -2340,9 +2348,9 @@
       <c r="T6" s="6"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
@@ -2362,940 +2370,940 @@
       <c r="T7" s="6"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="25"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="26"/>
     </row>
     <row r="9" ht="36.9" customHeight="1">
-      <c r="A9" t="s" s="29">
+      <c r="A9" t="s" s="30">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s" s="31">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s" s="31">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s" s="31">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s" s="31">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s" s="31">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s" s="31">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s" s="31">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s" s="31">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s" s="31">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s" s="31">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="O9" t="s" s="31">
+        <v>20</v>
+      </c>
+      <c r="P9" t="s" s="31">
+        <v>21</v>
+      </c>
+      <c r="Q9" t="s" s="31">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s" s="31">
+        <v>23</v>
+      </c>
+      <c r="S9" t="s" s="31">
+        <v>24</v>
+      </c>
+      <c r="T9" t="s" s="31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" ht="131.55" customHeight="1">
+      <c r="A10" s="32">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s" s="33">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s" s="34">
+        <v>29</v>
+      </c>
+      <c r="F10" s="35">
+        <v>44977</v>
+      </c>
+      <c r="G10" t="s" s="36">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s" s="36">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s" s="36">
+        <v>32</v>
+      </c>
+      <c r="J10" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="40"/>
+      <c r="T10" t="s" s="41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" ht="131.55" customHeight="1">
+      <c r="A11" s="32">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s" s="33">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s" s="34">
+        <v>36</v>
+      </c>
+      <c r="F11" s="35">
+        <v>44977</v>
+      </c>
+      <c r="G11" t="s" s="36">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s" s="36">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s" s="36">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="40"/>
+      <c r="T11" t="s" s="41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" ht="131.55" customHeight="1">
+      <c r="A12" s="32">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s" s="33">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s" s="34">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35">
+        <v>44977</v>
+      </c>
+      <c r="G12" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s" s="36">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s" s="36">
+        <v>44</v>
+      </c>
+      <c r="J12" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="40"/>
+      <c r="T12" t="s" s="41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" ht="131.55" customHeight="1">
+      <c r="A13" s="32">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s" s="33">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s" s="34">
+        <v>46</v>
+      </c>
+      <c r="F13" s="35">
+        <v>44979</v>
+      </c>
+      <c r="G13" t="s" s="36">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s" s="36">
+        <v>48</v>
+      </c>
+      <c r="I13" t="s" s="36">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="40"/>
+      <c r="T13" t="s" s="41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" ht="131.55" customHeight="1">
+      <c r="A14" s="32">
         <v>5</v>
       </c>
-      <c r="B9" t="s" s="30">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s" s="30">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s" s="30">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s" s="30">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s" s="30">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s" s="30">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s" s="30">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s" s="30">
-        <v>13</v>
-      </c>
-      <c r="J9" t="s" s="30">
-        <v>14</v>
-      </c>
-      <c r="K9" t="s" s="30">
-        <v>15</v>
-      </c>
-      <c r="L9" t="s" s="30">
-        <v>16</v>
-      </c>
-      <c r="M9" t="s" s="30">
-        <v>17</v>
-      </c>
-      <c r="N9" t="s" s="30">
-        <v>18</v>
-      </c>
-      <c r="O9" t="s" s="30">
-        <v>19</v>
-      </c>
-      <c r="P9" t="s" s="30">
-        <v>20</v>
-      </c>
-      <c r="Q9" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="R9" t="s" s="30">
-        <v>22</v>
-      </c>
-      <c r="S9" t="s" s="30">
-        <v>23</v>
-      </c>
-      <c r="T9" t="s" s="30">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" ht="131.55" customHeight="1">
-      <c r="A10" s="31">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="32">
+      <c r="B14" t="s" s="33">
         <v>26</v>
       </c>
-      <c r="D10" t="s" s="32">
+      <c r="C14" t="s" s="33">
         <v>27</v>
       </c>
-      <c r="E10" t="s" s="33">
+      <c r="D14" t="s" s="33">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="F14" s="35">
+        <v>44977</v>
+      </c>
+      <c r="G14" t="s" s="36">
+        <v>52</v>
+      </c>
+      <c r="H14" t="s" s="36">
+        <v>53</v>
+      </c>
+      <c r="I14" t="s" s="36">
+        <v>54</v>
+      </c>
+      <c r="J14" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="40"/>
+      <c r="T14" t="s" s="41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" ht="92.55" customHeight="1">
+      <c r="A15" s="32">
         <v>28</v>
       </c>
-      <c r="F10" s="34">
-        <v>44977</v>
-      </c>
-      <c r="G10" t="s" s="35">
-        <v>29</v>
-      </c>
-      <c r="H10" t="s" s="35">
-        <v>30</v>
-      </c>
-      <c r="I10" t="s" s="35">
-        <v>31</v>
-      </c>
-      <c r="J10" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="39"/>
-      <c r="T10" t="s" s="40">
+      <c r="B15" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s" s="33">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s" s="42">
+        <v>56</v>
+      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K15" t="s" s="37">
+        <v>58</v>
+      </c>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="40"/>
+      <c r="T15" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" ht="105.55" customHeight="1">
+      <c r="A16" s="32">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s" s="33">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s" s="42">
+        <v>61</v>
+      </c>
+      <c r="F16" s="35">
+        <v>44991</v>
+      </c>
+      <c r="G16" t="s" s="36">
+        <v>62</v>
+      </c>
+      <c r="H16" t="s" s="36">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s" s="36">
+        <v>64</v>
+      </c>
+      <c r="J16" t="s" s="37">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" ht="131.55" customHeight="1">
-      <c r="A11" s="31">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="32">
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
+      <c r="P16" t="s" s="37">
+        <v>65</v>
+      </c>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="40"/>
+      <c r="T16" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" ht="40.55" customHeight="1">
+      <c r="A17" s="32">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s" s="33">
         <v>26</v>
       </c>
-      <c r="D11" t="s" s="32">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s" s="33">
-        <v>35</v>
-      </c>
-      <c r="F11" s="34">
-        <v>44977</v>
-      </c>
-      <c r="G11" t="s" s="35">
-        <v>36</v>
-      </c>
-      <c r="H11" t="s" s="35">
-        <v>37</v>
-      </c>
-      <c r="I11" t="s" s="35">
-        <v>38</v>
-      </c>
-      <c r="J11" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K11" s="37"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="39"/>
-      <c r="T11" t="s" s="40">
+      <c r="C17" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s" s="33">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s" s="34">
+        <v>67</v>
+      </c>
+      <c r="F17" s="43">
+        <v>44981</v>
+      </c>
+      <c r="G17" t="s" s="44">
+        <v>68</v>
+      </c>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" t="s" s="37">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" ht="131.55" customHeight="1">
-      <c r="A12" s="31">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="32">
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
+      <c r="P17" t="s" s="37">
+        <v>69</v>
+      </c>
+      <c r="Q17" s="39"/>
+      <c r="R17" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="S17" s="40"/>
+      <c r="T17" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" ht="105.55" customHeight="1">
+      <c r="A18" s="32">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s" s="33">
         <v>26</v>
       </c>
-      <c r="D12" t="s" s="32">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s" s="33">
-        <v>40</v>
-      </c>
-      <c r="F12" s="34">
-        <v>44977</v>
-      </c>
-      <c r="G12" t="s" s="35">
-        <v>41</v>
-      </c>
-      <c r="H12" t="s" s="35">
-        <v>42</v>
-      </c>
-      <c r="I12" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="J12" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="39"/>
-      <c r="T12" t="s" s="40">
+      <c r="C18" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s" s="33">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s" s="34">
+        <v>71</v>
+      </c>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s" s="37">
+        <v>72</v>
+      </c>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="40"/>
+      <c r="T18" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" ht="105.55" customHeight="1">
+      <c r="A19" s="32">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s" s="33">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s" s="34">
+        <v>74</v>
+      </c>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s" s="37">
+        <v>75</v>
+      </c>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="40"/>
+      <c r="T19" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" ht="209.55" customHeight="1">
+      <c r="A20" s="32">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s" s="33">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s" s="34">
+        <v>77</v>
+      </c>
+      <c r="F20" s="35">
+        <v>44981</v>
+      </c>
+      <c r="G20" t="s" s="36">
+        <v>78</v>
+      </c>
+      <c r="H20" t="s" s="36">
+        <v>79</v>
+      </c>
+      <c r="I20" t="s" s="36">
+        <v>80</v>
+      </c>
+      <c r="J20" t="s" s="37">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" ht="131.55" customHeight="1">
-      <c r="A13" s="31">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="32">
+      <c r="K20" s="38"/>
+      <c r="L20" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="M20" t="s" s="48">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s" s="49">
+        <v>81</v>
+      </c>
+      <c r="O20" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="P20" t="s" s="37">
+        <v>82</v>
+      </c>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="40"/>
+      <c r="T20" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" ht="183.55" customHeight="1">
+      <c r="A21" s="32">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s" s="33">
         <v>26</v>
       </c>
-      <c r="D13" t="s" s="32">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s" s="33">
-        <v>45</v>
-      </c>
-      <c r="F13" s="34">
-        <v>44979</v>
-      </c>
-      <c r="G13" t="s" s="35">
-        <v>46</v>
-      </c>
-      <c r="H13" t="s" s="35">
-        <v>47</v>
-      </c>
-      <c r="I13" t="s" s="35">
-        <v>48</v>
-      </c>
-      <c r="J13" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K13" s="37"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="39"/>
-      <c r="T13" t="s" s="40">
+      <c r="C21" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s" s="33">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s" s="34">
+        <v>84</v>
+      </c>
+      <c r="F21" s="35">
+        <v>44981</v>
+      </c>
+      <c r="G21" t="s" s="36">
+        <v>85</v>
+      </c>
+      <c r="H21" t="s" s="44">
+        <v>86</v>
+      </c>
+      <c r="I21" t="s" s="44">
+        <v>87</v>
+      </c>
+      <c r="J21" t="s" s="37">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" ht="131.55" customHeight="1">
-      <c r="A14" s="31">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="32">
+      <c r="K21" s="38"/>
+      <c r="L21" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="M21" t="s" s="48">
+        <v>33</v>
+      </c>
+      <c r="N21" t="s" s="50">
+        <v>88</v>
+      </c>
+      <c r="O21" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="P21" t="s" s="37">
+        <v>89</v>
+      </c>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="40"/>
+      <c r="T21" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" ht="105.55" customHeight="1">
+      <c r="A22" s="32">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s" s="33">
         <v>26</v>
       </c>
-      <c r="D14" t="s" s="32">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s" s="33">
-        <v>50</v>
-      </c>
-      <c r="F14" s="34">
-        <v>44977</v>
-      </c>
-      <c r="G14" t="s" s="35">
-        <v>51</v>
-      </c>
-      <c r="H14" t="s" s="35">
-        <v>52</v>
-      </c>
-      <c r="I14" t="s" s="35">
-        <v>53</v>
-      </c>
-      <c r="J14" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K14" s="37"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="39"/>
-      <c r="T14" t="s" s="40">
+      <c r="C22" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s" s="33">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s" s="34">
+        <v>91</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K22" t="s" s="37">
+        <v>72</v>
+      </c>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="40"/>
+      <c r="T22" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" ht="105.55" customHeight="1">
+      <c r="A23" s="32">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s" s="33">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s" s="34">
+        <v>93</v>
+      </c>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K23" t="s" s="37">
+        <v>72</v>
+      </c>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="40"/>
+      <c r="T23" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" ht="105.55" customHeight="1">
+      <c r="A24" s="32">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s" s="33">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s" s="34">
+        <v>95</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K24" t="s" s="37">
+        <v>96</v>
+      </c>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="40"/>
+      <c r="T24" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" ht="105.55" customHeight="1">
+      <c r="A25" s="32">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s" s="33">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s" s="34">
+        <v>98</v>
+      </c>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K25" t="s" s="37">
+        <v>72</v>
+      </c>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="40"/>
+      <c r="T25" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" ht="105.55" customHeight="1">
+      <c r="A26" s="32">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s" s="33">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s" s="34">
+        <v>100</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="K26" t="s" s="37">
+        <v>101</v>
+      </c>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="40"/>
+      <c r="T26" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" ht="404.55" customHeight="1">
+      <c r="A27" s="32">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s" s="33">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s" s="34">
+        <v>103</v>
+      </c>
+      <c r="F27" s="35">
+        <v>44981</v>
+      </c>
+      <c r="G27" t="s" s="36">
+        <v>104</v>
+      </c>
+      <c r="H27" t="s" s="36">
+        <v>105</v>
+      </c>
+      <c r="I27" t="s" s="44">
+        <v>106</v>
+      </c>
+      <c r="J27" t="s" s="37">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" ht="92.55" customHeight="1">
-      <c r="A15" s="31">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="32">
+      <c r="K27" s="38"/>
+      <c r="L27" t="s" s="37">
+        <v>33</v>
+      </c>
+      <c r="M27" t="s" s="48">
+        <v>33</v>
+      </c>
+      <c r="N27" t="s" s="51">
+        <v>107</v>
+      </c>
+      <c r="O27" t="s" s="37">
+        <v>57</v>
+      </c>
+      <c r="P27" t="s" s="37">
+        <v>108</v>
+      </c>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="40"/>
+      <c r="T27" t="s" s="41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" ht="183.05" customHeight="1">
+      <c r="A28" s="52">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s" s="53">
         <v>26</v>
       </c>
-      <c r="D15" t="s" s="32">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s" s="41">
-        <v>55</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K15" t="s" s="36">
+      <c r="C28" t="s" s="53">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s" s="53">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s" s="54">
+        <v>110</v>
+      </c>
+      <c r="F28" s="43">
+        <v>44981</v>
+      </c>
+      <c r="G28" t="s" s="44">
+        <v>111</v>
+      </c>
+      <c r="H28" t="s" s="55">
+        <v>112</v>
+      </c>
+      <c r="I28" t="s" s="56">
+        <v>113</v>
+      </c>
+      <c r="J28" t="s" s="57">
+        <v>33</v>
+      </c>
+      <c r="K28" s="47"/>
+      <c r="L28" t="s" s="57">
+        <v>33</v>
+      </c>
+      <c r="M28" t="s" s="57">
+        <v>33</v>
+      </c>
+      <c r="N28" t="s" s="55">
+        <v>114</v>
+      </c>
+      <c r="O28" t="s" s="57">
         <v>57</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="39"/>
-      <c r="T15" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" ht="105.55" customHeight="1">
-      <c r="A16" s="31">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="32">
+      <c r="P28" t="s" s="57">
+        <v>115</v>
+      </c>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="59"/>
+      <c r="T28" t="s" s="60">
         <v>59</v>
       </c>
-      <c r="E16" t="s" s="41">
-        <v>60</v>
-      </c>
-      <c r="F16" s="34">
-        <v>44981</v>
-      </c>
-      <c r="G16" t="s" s="35">
-        <v>61</v>
-      </c>
-      <c r="H16" t="s" s="35">
-        <v>62</v>
-      </c>
-      <c r="I16" t="s" s="35">
-        <v>63</v>
-      </c>
-      <c r="J16" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="38"/>
-      <c r="P16" t="s" s="36">
-        <v>64</v>
-      </c>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="39"/>
-      <c r="T16" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" ht="40.55" customHeight="1">
-      <c r="A17" s="31">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s" s="32">
-        <v>65</v>
-      </c>
-      <c r="E17" t="s" s="33">
-        <v>66</v>
-      </c>
-      <c r="F17" s="42">
-        <v>44981</v>
-      </c>
-      <c r="G17" t="s" s="43">
-        <v>67</v>
-      </c>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K17" s="37"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="38"/>
-      <c r="P17" t="s" s="36">
-        <v>68</v>
-      </c>
-      <c r="Q17" s="38"/>
-      <c r="R17" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="S17" s="39"/>
-      <c r="T17" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" ht="105.55" customHeight="1">
-      <c r="A18" s="31">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s" s="32">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s" s="33">
-        <v>70</v>
-      </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K18" t="s" s="36">
-        <v>71</v>
-      </c>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="39"/>
-      <c r="T18" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" ht="105.55" customHeight="1">
-      <c r="A19" s="31">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s" s="32">
-        <v>72</v>
-      </c>
-      <c r="E19" t="s" s="33">
-        <v>73</v>
-      </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K19" t="s" s="36">
-        <v>74</v>
-      </c>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="39"/>
-      <c r="T19" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" ht="209.55" customHeight="1">
-      <c r="A20" s="31">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s" s="32">
-        <v>75</v>
-      </c>
-      <c r="E20" t="s" s="33">
-        <v>76</v>
-      </c>
-      <c r="F20" s="34">
-        <v>44981</v>
-      </c>
-      <c r="G20" t="s" s="35">
-        <v>77</v>
-      </c>
-      <c r="H20" t="s" s="35">
-        <v>78</v>
-      </c>
-      <c r="I20" t="s" s="35">
-        <v>79</v>
-      </c>
-      <c r="J20" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K20" s="37"/>
-      <c r="L20" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="M20" t="s" s="47">
-        <v>56</v>
-      </c>
-      <c r="N20" t="s" s="48">
-        <v>80</v>
-      </c>
-      <c r="O20" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="P20" t="s" s="36">
-        <v>81</v>
-      </c>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="39"/>
-      <c r="T20" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" ht="183.55" customHeight="1">
-      <c r="A21" s="31">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s" s="32">
-        <v>82</v>
-      </c>
-      <c r="E21" t="s" s="33">
-        <v>83</v>
-      </c>
-      <c r="F21" s="34">
-        <v>44981</v>
-      </c>
-      <c r="G21" t="s" s="35">
-        <v>84</v>
-      </c>
-      <c r="H21" t="s" s="43">
-        <v>85</v>
-      </c>
-      <c r="I21" t="s" s="43">
-        <v>86</v>
-      </c>
-      <c r="J21" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K21" s="37"/>
-      <c r="L21" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="M21" t="s" s="47">
-        <v>32</v>
-      </c>
-      <c r="N21" t="s" s="49">
-        <v>87</v>
-      </c>
-      <c r="O21" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="P21" t="s" s="36">
-        <v>88</v>
-      </c>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="39"/>
-      <c r="T21" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" ht="105.55" customHeight="1">
-      <c r="A22" s="31">
-        <v>56</v>
-      </c>
-      <c r="B22" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s" s="32">
-        <v>89</v>
-      </c>
-      <c r="E22" t="s" s="33">
-        <v>90</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K22" t="s" s="36">
-        <v>71</v>
-      </c>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="39"/>
-      <c r="T22" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" ht="105.55" customHeight="1">
-      <c r="A23" s="31">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s" s="32">
-        <v>91</v>
-      </c>
-      <c r="E23" t="s" s="33">
-        <v>92</v>
-      </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K23" t="s" s="36">
-        <v>71</v>
-      </c>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="39"/>
-      <c r="T23" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" ht="105.55" customHeight="1">
-      <c r="A24" s="31">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D24" t="s" s="32">
-        <v>93</v>
-      </c>
-      <c r="E24" t="s" s="33">
-        <v>94</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K24" t="s" s="36">
-        <v>95</v>
-      </c>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="39"/>
-      <c r="T24" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" ht="105.55" customHeight="1">
-      <c r="A25" s="31">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D25" t="s" s="32">
-        <v>96</v>
-      </c>
-      <c r="E25" t="s" s="33">
-        <v>97</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K25" t="s" s="36">
-        <v>71</v>
-      </c>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="39"/>
-      <c r="T25" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" ht="105.55" customHeight="1">
-      <c r="A26" s="31">
-        <v>60</v>
-      </c>
-      <c r="B26" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s" s="32">
-        <v>98</v>
-      </c>
-      <c r="E26" t="s" s="33">
-        <v>99</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="K26" t="s" s="36">
-        <v>100</v>
-      </c>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="39"/>
-      <c r="T26" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" ht="404.55" customHeight="1">
-      <c r="A27" s="31">
-        <v>61</v>
-      </c>
-      <c r="B27" t="s" s="32">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s" s="32">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s" s="32">
-        <v>101</v>
-      </c>
-      <c r="E27" t="s" s="33">
-        <v>102</v>
-      </c>
-      <c r="F27" s="34">
-        <v>44981</v>
-      </c>
-      <c r="G27" t="s" s="35">
-        <v>103</v>
-      </c>
-      <c r="H27" t="s" s="35">
-        <v>104</v>
-      </c>
-      <c r="I27" t="s" s="43">
-        <v>105</v>
-      </c>
-      <c r="J27" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="K27" s="37"/>
-      <c r="L27" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="M27" t="s" s="47">
-        <v>32</v>
-      </c>
-      <c r="N27" t="s" s="50">
-        <v>106</v>
-      </c>
-      <c r="O27" t="s" s="36">
-        <v>56</v>
-      </c>
-      <c r="P27" t="s" s="36">
-        <v>107</v>
-      </c>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="39"/>
-      <c r="T27" t="s" s="40">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" ht="183.05" customHeight="1">
-      <c r="A28" s="51">
-        <v>62</v>
-      </c>
-      <c r="B28" t="s" s="52">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s" s="52">
-        <v>26</v>
-      </c>
-      <c r="D28" t="s" s="52">
-        <v>108</v>
-      </c>
-      <c r="E28" t="s" s="53">
-        <v>109</v>
-      </c>
-      <c r="F28" s="42">
-        <v>44981</v>
-      </c>
-      <c r="G28" t="s" s="43">
-        <v>110</v>
-      </c>
-      <c r="H28" t="s" s="54">
-        <v>111</v>
-      </c>
-      <c r="I28" t="s" s="55">
-        <v>112</v>
-      </c>
-      <c r="J28" t="s" s="56">
-        <v>32</v>
-      </c>
-      <c r="K28" s="46"/>
-      <c r="L28" t="s" s="56">
-        <v>32</v>
-      </c>
-      <c r="M28" t="s" s="56">
-        <v>32</v>
-      </c>
-      <c r="N28" t="s" s="54">
-        <v>113</v>
-      </c>
-      <c r="O28" t="s" s="56">
-        <v>56</v>
-      </c>
-      <c r="P28" t="s" s="56">
-        <v>114</v>
-      </c>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="58"/>
-      <c r="T28" t="s" s="59">
-        <v>58</v>
-      </c>
     </row>
     <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="63"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="62"/>
-      <c r="R29" s="64"/>
-      <c r="S29" s="65"/>
-      <c r="T29" s="62"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+      <c r="R29" s="65"/>
+      <c r="S29" s="66"/>
+      <c r="T29" s="63"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="3"/>

</xml_diff>

<commit_message>
Corretti errori caso ID 4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LIS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LIS/V.2.0/report-checklist.xlsx
@@ -189,13 +189,13 @@
 </t>
   </si>
   <si>
-    <t>16:20:00</t>
+    <t>14:50:00</t>
   </si>
   <si>
-    <t>f22259c49de5fd81</t>
+    <t xml:space="preserve">30a7b8ad002098a7 </t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.8d2c41354c3031c113f1691db097b7dfa8b9145e3722183ab576c7ea1c254059.5115a94cae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.8d2c41354c3031c113f1691db097b7dfa8b9145e3722183ab576c7ea1c254059.37ac173c65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -878,7 +878,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1004,6 +1004,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2605,15 +2608,15 @@
         <v>46</v>
       </c>
       <c r="F13" s="35">
-        <v>44979</v>
+        <v>45006</v>
       </c>
       <c r="G13" t="s" s="36">
         <v>47</v>
       </c>
-      <c r="H13" t="s" s="36">
+      <c r="H13" t="s" s="42">
         <v>48</v>
       </c>
-      <c r="I13" t="s" s="36">
+      <c r="I13" t="s" s="42">
         <v>49</v>
       </c>
       <c r="J13" t="s" s="37">
@@ -2689,7 +2692,7 @@
       <c r="D15" t="s" s="33">
         <v>55</v>
       </c>
-      <c r="E15" t="s" s="42">
+      <c r="E15" t="s" s="43">
         <v>56</v>
       </c>
       <c r="F15" s="35"/>
@@ -2727,7 +2730,7 @@
       <c r="D16" t="s" s="33">
         <v>60</v>
       </c>
-      <c r="E16" t="s" s="42">
+      <c r="E16" t="s" s="43">
         <v>61</v>
       </c>
       <c r="F16" s="35">
@@ -2784,10 +2787,10 @@
       <c r="E17" t="s" s="34">
         <v>68</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="44">
         <v>44981</v>
       </c>
-      <c r="G17" t="s" s="44">
+      <c r="G17" t="s" s="45">
         <v>69</v>
       </c>
       <c r="H17" s="35"/>
@@ -2828,8 +2831,8 @@
       <c r="E18" t="s" s="34">
         <v>72</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
       <c r="J18" t="s" s="37">
@@ -2878,7 +2881,7 @@
       </c>
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
-      <c r="N19" s="47"/>
+      <c r="N19" s="48"/>
       <c r="O19" s="39"/>
       <c r="P19" s="38"/>
       <c r="Q19" s="39"/>
@@ -2923,10 +2926,10 @@
       <c r="L20" t="s" s="37">
         <v>33</v>
       </c>
-      <c r="M20" t="s" s="48">
+      <c r="M20" t="s" s="49">
         <v>57</v>
       </c>
-      <c r="N20" t="s" s="49">
+      <c r="N20" t="s" s="50">
         <v>82</v>
       </c>
       <c r="O20" t="s" s="37">
@@ -2964,10 +2967,10 @@
       <c r="G21" t="s" s="36">
         <v>86</v>
       </c>
-      <c r="H21" t="s" s="44">
+      <c r="H21" t="s" s="45">
         <v>87</v>
       </c>
-      <c r="I21" t="s" s="44">
+      <c r="I21" t="s" s="45">
         <v>88</v>
       </c>
       <c r="J21" t="s" s="37">
@@ -2977,10 +2980,10 @@
       <c r="L21" t="s" s="37">
         <v>33</v>
       </c>
-      <c r="M21" t="s" s="48">
+      <c r="M21" t="s" s="49">
         <v>33</v>
       </c>
-      <c r="N21" t="s" s="50">
+      <c r="N21" t="s" s="51">
         <v>89</v>
       </c>
       <c r="O21" t="s" s="37">
@@ -3014,8 +3017,8 @@
       </c>
       <c r="F22" s="35"/>
       <c r="G22" s="36"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
       <c r="J22" t="s" s="37">
         <v>57</v>
       </c>
@@ -3176,7 +3179,7 @@
       </c>
       <c r="L26" s="39"/>
       <c r="M26" s="39"/>
-      <c r="N26" s="47"/>
+      <c r="N26" s="48"/>
       <c r="O26" s="39"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="39"/>
@@ -3211,7 +3214,7 @@
       <c r="H27" t="s" s="36">
         <v>106</v>
       </c>
-      <c r="I27" t="s" s="44">
+      <c r="I27" t="s" s="45">
         <v>107</v>
       </c>
       <c r="J27" t="s" s="37">
@@ -3221,10 +3224,10 @@
       <c r="L27" t="s" s="37">
         <v>33</v>
       </c>
-      <c r="M27" t="s" s="48">
+      <c r="M27" t="s" s="49">
         <v>33</v>
       </c>
-      <c r="N27" t="s" s="51">
+      <c r="N27" t="s" s="52">
         <v>108</v>
       </c>
       <c r="O27" t="s" s="37">
@@ -3241,56 +3244,56 @@
       </c>
     </row>
     <row r="28" ht="183.05" customHeight="1">
-      <c r="A28" s="52">
+      <c r="A28" s="53">
         <v>62</v>
       </c>
-      <c r="B28" t="s" s="53">
+      <c r="B28" t="s" s="54">
         <v>26</v>
       </c>
-      <c r="C28" t="s" s="53">
+      <c r="C28" t="s" s="54">
         <v>27</v>
       </c>
-      <c r="D28" t="s" s="53">
+      <c r="D28" t="s" s="54">
         <v>110</v>
       </c>
-      <c r="E28" t="s" s="54">
+      <c r="E28" t="s" s="55">
         <v>111</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="44">
         <v>44981</v>
       </c>
-      <c r="G28" t="s" s="44">
+      <c r="G28" t="s" s="45">
         <v>112</v>
       </c>
-      <c r="H28" t="s" s="55">
+      <c r="H28" t="s" s="56">
         <v>113</v>
       </c>
-      <c r="I28" t="s" s="56">
+      <c r="I28" t="s" s="57">
         <v>114</v>
       </c>
-      <c r="J28" t="s" s="57">
+      <c r="J28" t="s" s="58">
         <v>33</v>
       </c>
-      <c r="K28" s="47"/>
-      <c r="L28" t="s" s="57">
+      <c r="K28" s="48"/>
+      <c r="L28" t="s" s="58">
         <v>33</v>
       </c>
-      <c r="M28" t="s" s="57">
+      <c r="M28" t="s" s="58">
         <v>33</v>
       </c>
-      <c r="N28" t="s" s="55">
+      <c r="N28" t="s" s="56">
         <v>115</v>
       </c>
-      <c r="O28" t="s" s="57">
+      <c r="O28" t="s" s="58">
         <v>57</v>
       </c>
-      <c r="P28" t="s" s="57">
+      <c r="P28" t="s" s="58">
         <v>116</v>
       </c>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="59"/>
-      <c r="T28" t="s" s="60">
+      <c r="Q28" s="59"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="60"/>
+      <c r="T28" t="s" s="61">
         <v>59</v>
       </c>
     </row>
@@ -3300,21 +3303,21 @@
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="65"/>
-      <c r="S29" s="66"/>
-      <c r="T29" s="63"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="65"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="67"/>
+      <c r="T29" s="64"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="3"/>

</xml_diff>

<commit_message>
Corretto errore caso test ID 4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LIS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-LIS/V.2.0/report-checklist.xlsx
@@ -51,7 +51,7 @@
     <t>subject_application_vendor: GESAN SRL</t>
   </si>
   <si>
-    <t>subject_application_version: v.2.0</t>
+    <t>subject_application_version: V.2.0</t>
   </si>
   <si>
     <t>ID</t>
@@ -129,13 +129,13 @@
 </t>
   </si>
   <si>
-    <t>16:30:00</t>
+    <t>14:13:00</t>
   </si>
   <si>
-    <t>5ecb60650c0bcfed</t>
+    <t>e7316a88c71fce30</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.f1e497be9949acc3f3de5928e179f0e15fd9febfe52158f4b6f02590c3a31589.289ab10712^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.f1e497be9949acc3f3de5928e179f0e15fd9febfe52158f4b6f02590c3a31589.30a5912885^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -153,13 +153,13 @@
 </t>
   </si>
   <si>
-    <t>17:20:00</t>
+    <t>14:15:00</t>
   </si>
   <si>
-    <t>aa0245665496c5ce</t>
+    <t>20cb01ba7aa5d4ac</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.91a04f98b62517bd632862929fd034ef2f2b0a7e0ac46a3363bf51af5361495c.fe29552064^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.91a04f98b62517bd632862929fd034ef2f2b0a7e0ac46a3363bf51af5361495c.49310c100a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -171,13 +171,13 @@
 </t>
   </si>
   <si>
-    <t>17:26:00</t>
+    <t>14:18:00</t>
   </si>
   <si>
-    <t>e0b270b48b02538e</t>
+    <t>1b4a7514f936557c</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.3b7338f182c6babeeb3400cf6ae52325ef95f74402d312c80f0619e0e9c47227.8628b78a96^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.3b7338f182c6babeeb3400cf6ae52325ef95f74402d312c80f0619e0e9c47227.56ffac1e11^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -189,13 +189,13 @@
 </t>
   </si>
   <si>
-    <t>14:50:00</t>
+    <t>13:30:00</t>
   </si>
   <si>
-    <t xml:space="preserve">30a7b8ad002098a7 </t>
+    <t xml:space="preserve">527c328f0d2cd011 </t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.8d2c41354c3031c113f1691db097b7dfa8b9145e3722183ab576c7ea1c254059.37ac173c65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.8d2c41354c3031c113f1691db097b7dfa8b9145e3722183ab576c7ea1c254059.1f77350c64^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -207,13 +207,13 @@
 </t>
   </si>
   <si>
-    <t>18:20:00</t>
+    <t>14:20:00</t>
   </si>
   <si>
-    <t>10efb441e8cabe0d</t>
+    <t>c3a8a36134a1b84d</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.532e6518844555ec4ffe1a8de85a3abbbdaf59b4d604eab98798ccd6755c7587.5f93218fb8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.532e6518844555ec4ffe1a8de85a3abbbdaf59b4d604eab98798ccd6755c7587.fa08c5d23d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
@@ -579,7 +579,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -789,6 +789,36 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
@@ -821,21 +851,6 @@
       </right>
       <top style="thin">
         <color indexed="10"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -878,7 +893,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1005,12 +1020,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="59" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1023,22 +1032,31 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1059,10 +1077,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2476,7 +2494,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="35">
-        <v>44977</v>
+        <v>45014</v>
       </c>
       <c r="G10" t="s" s="36">
         <v>30</v>
@@ -2520,7 +2538,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="35">
-        <v>44977</v>
+        <v>45014</v>
       </c>
       <c r="G11" t="s" s="36">
         <v>37</v>
@@ -2563,16 +2581,16 @@
       <c r="E12" t="s" s="34">
         <v>41</v>
       </c>
-      <c r="F12" s="35">
-        <v>44977</v>
-      </c>
-      <c r="G12" t="s" s="36">
+      <c r="F12" s="42">
+        <v>45014</v>
+      </c>
+      <c r="G12" t="s" s="43">
         <v>42</v>
       </c>
-      <c r="H12" t="s" s="36">
+      <c r="H12" t="s" s="43">
         <v>43</v>
       </c>
-      <c r="I12" t="s" s="36">
+      <c r="I12" t="s" s="43">
         <v>44</v>
       </c>
       <c r="J12" t="s" s="37">
@@ -2607,16 +2625,16 @@
       <c r="E13" t="s" s="34">
         <v>46</v>
       </c>
-      <c r="F13" s="35">
-        <v>45006</v>
-      </c>
-      <c r="G13" t="s" s="36">
+      <c r="F13" s="44">
+        <v>45014</v>
+      </c>
+      <c r="G13" t="s" s="45">
         <v>47</v>
       </c>
-      <c r="H13" t="s" s="42">
+      <c r="H13" t="s" s="46">
         <v>48</v>
       </c>
-      <c r="I13" t="s" s="42">
+      <c r="I13" t="s" s="47">
         <v>49</v>
       </c>
       <c r="J13" t="s" s="37">
@@ -2651,16 +2669,16 @@
       <c r="E14" t="s" s="34">
         <v>51</v>
       </c>
-      <c r="F14" s="35">
-        <v>44977</v>
+      <c r="F14" s="42">
+        <v>45014</v>
       </c>
       <c r="G14" t="s" s="36">
         <v>52</v>
       </c>
-      <c r="H14" t="s" s="36">
+      <c r="H14" t="s" s="43">
         <v>53</v>
       </c>
-      <c r="I14" t="s" s="36">
+      <c r="I14" t="s" s="43">
         <v>54</v>
       </c>
       <c r="J14" t="s" s="37">
@@ -2692,13 +2710,13 @@
       <c r="D15" t="s" s="33">
         <v>55</v>
       </c>
-      <c r="E15" t="s" s="43">
+      <c r="E15" t="s" s="48">
         <v>56</v>
       </c>
-      <c r="F15" s="35"/>
+      <c r="F15" s="44"/>
       <c r="G15" s="36"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" t="s" s="37">
         <v>57</v>
       </c>
@@ -2730,7 +2748,7 @@
       <c r="D16" t="s" s="33">
         <v>60</v>
       </c>
-      <c r="E16" t="s" s="43">
+      <c r="E16" t="s" s="48">
         <v>61</v>
       </c>
       <c r="F16" s="35">
@@ -2787,10 +2805,10 @@
       <c r="E17" t="s" s="34">
         <v>68</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="42">
         <v>44981</v>
       </c>
-      <c r="G17" t="s" s="45">
+      <c r="G17" t="s" s="43">
         <v>69</v>
       </c>
       <c r="H17" s="35"/>
@@ -2831,8 +2849,8 @@
       <c r="E18" t="s" s="34">
         <v>72</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
       <c r="J18" t="s" s="37">
@@ -2881,7 +2899,7 @@
       </c>
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
-      <c r="N19" s="48"/>
+      <c r="N19" s="49"/>
       <c r="O19" s="39"/>
       <c r="P19" s="38"/>
       <c r="Q19" s="39"/>
@@ -2926,10 +2944,10 @@
       <c r="L20" t="s" s="37">
         <v>33</v>
       </c>
-      <c r="M20" t="s" s="49">
+      <c r="M20" t="s" s="50">
         <v>57</v>
       </c>
-      <c r="N20" t="s" s="50">
+      <c r="N20" t="s" s="51">
         <v>82</v>
       </c>
       <c r="O20" t="s" s="37">
@@ -2967,10 +2985,10 @@
       <c r="G21" t="s" s="36">
         <v>86</v>
       </c>
-      <c r="H21" t="s" s="45">
+      <c r="H21" t="s" s="43">
         <v>87</v>
       </c>
-      <c r="I21" t="s" s="45">
+      <c r="I21" t="s" s="43">
         <v>88</v>
       </c>
       <c r="J21" t="s" s="37">
@@ -2980,10 +2998,10 @@
       <c r="L21" t="s" s="37">
         <v>33</v>
       </c>
-      <c r="M21" t="s" s="49">
+      <c r="M21" t="s" s="50">
         <v>33</v>
       </c>
-      <c r="N21" t="s" s="51">
+      <c r="N21" t="s" s="52">
         <v>89</v>
       </c>
       <c r="O21" t="s" s="37">
@@ -3017,8 +3035,8 @@
       </c>
       <c r="F22" s="35"/>
       <c r="G22" s="36"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
       <c r="J22" t="s" s="37">
         <v>57</v>
       </c>
@@ -3179,7 +3197,7 @@
       </c>
       <c r="L26" s="39"/>
       <c r="M26" s="39"/>
-      <c r="N26" s="48"/>
+      <c r="N26" s="49"/>
       <c r="O26" s="39"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="39"/>
@@ -3214,7 +3232,7 @@
       <c r="H27" t="s" s="36">
         <v>106</v>
       </c>
-      <c r="I27" t="s" s="45">
+      <c r="I27" t="s" s="43">
         <v>107</v>
       </c>
       <c r="J27" t="s" s="37">
@@ -3224,10 +3242,10 @@
       <c r="L27" t="s" s="37">
         <v>33</v>
       </c>
-      <c r="M27" t="s" s="49">
+      <c r="M27" t="s" s="50">
         <v>33</v>
       </c>
-      <c r="N27" t="s" s="52">
+      <c r="N27" t="s" s="53">
         <v>108</v>
       </c>
       <c r="O27" t="s" s="37">
@@ -3244,56 +3262,56 @@
       </c>
     </row>
     <row r="28" ht="183.05" customHeight="1">
-      <c r="A28" s="53">
+      <c r="A28" s="54">
         <v>62</v>
       </c>
-      <c r="B28" t="s" s="54">
+      <c r="B28" t="s" s="55">
         <v>26</v>
       </c>
-      <c r="C28" t="s" s="54">
+      <c r="C28" t="s" s="55">
         <v>27</v>
       </c>
-      <c r="D28" t="s" s="54">
+      <c r="D28" t="s" s="55">
         <v>110</v>
       </c>
-      <c r="E28" t="s" s="55">
+      <c r="E28" t="s" s="56">
         <v>111</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="42">
         <v>44981</v>
       </c>
-      <c r="G28" t="s" s="45">
+      <c r="G28" t="s" s="43">
         <v>112</v>
       </c>
-      <c r="H28" t="s" s="56">
+      <c r="H28" t="s" s="57">
         <v>113</v>
       </c>
-      <c r="I28" t="s" s="57">
+      <c r="I28" t="s" s="58">
         <v>114</v>
       </c>
-      <c r="J28" t="s" s="58">
+      <c r="J28" t="s" s="59">
         <v>33</v>
       </c>
-      <c r="K28" s="48"/>
-      <c r="L28" t="s" s="58">
+      <c r="K28" s="49"/>
+      <c r="L28" t="s" s="59">
         <v>33</v>
       </c>
-      <c r="M28" t="s" s="58">
+      <c r="M28" t="s" s="59">
         <v>33</v>
       </c>
-      <c r="N28" t="s" s="56">
+      <c r="N28" t="s" s="57">
         <v>115</v>
       </c>
-      <c r="O28" t="s" s="58">
+      <c r="O28" t="s" s="59">
         <v>57</v>
       </c>
-      <c r="P28" t="s" s="58">
+      <c r="P28" t="s" s="59">
         <v>116</v>
       </c>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="60"/>
-      <c r="T28" t="s" s="61">
+      <c r="Q28" s="60"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="61"/>
+      <c r="T28" t="s" s="62">
         <v>59</v>
       </c>
     </row>
@@ -3303,21 +3321,21 @@
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="65"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="65"/>
-      <c r="P29" s="64"/>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="66"/>
-      <c r="S29" s="67"/>
-      <c r="T29" s="64"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="66"/>
+      <c r="N29" s="65"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="65"/>
+      <c r="R29" s="67"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="65"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="3"/>

</xml_diff>